<commit_message>
commented out pie charts, need to fix
</commit_message>
<xml_diff>
--- a/vgat_oprm1_subcellular_metrics.xlsx
+++ b/vgat_oprm1_subcellular_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO32"/>
+  <dimension ref="A1:AP32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,25 +616,30 @@
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
+          <t>Total Cell Count</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
           <t>Subcellular cluster: Channel 2: Area (vgat_Neg: oprm1_Neg)</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Subcellular cluster: Channel 2: Mean channel intensity (vgat_Neg: oprm1_Neg)</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Subcellular: Channel 2: Num spots estimated (vgat_Neg: oprm1_Neg)</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Subcellular: Channel 2: Num single spots (vgat_Neg: oprm1_Neg)</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Subcellular: Channel 2: Num clusters (vgat_Neg: oprm1_Neg)</t>
         </is>
@@ -656,7 +661,7 @@
         <v>0.1268012969</v>
       </c>
       <c r="E2" t="n">
-        <v>11.83545826317056</v>
+        <v>8.804581245526128</v>
       </c>
       <c r="F2" t="n">
         <v>484.7928776422764</v>
@@ -671,7 +676,7 @@
         <v>0.0195548698</v>
       </c>
       <c r="J2" t="n">
-        <v>84.60428193408708</v>
+        <v>62.93843951324266</v>
       </c>
       <c r="K2" t="n">
         <v>103.20150875</v>
@@ -686,7 +691,7 @@
         <v>0.0380905447</v>
       </c>
       <c r="O2" t="n">
-        <v>3.560259802742363</v>
+        <v>2.648532569792412</v>
       </c>
       <c r="P2" t="n">
         <v>7758.338379352638</v>
@@ -698,7 +703,7 @@
         <v>0.3886457692</v>
       </c>
       <c r="S2" t="n">
-        <v>34.42386336300217</v>
+        <v>25.6084466714388</v>
       </c>
       <c r="T2" t="n">
         <v>0.1844467114</v>
@@ -752,18 +757,21 @@
         <v>532</v>
       </c>
       <c r="AK2" t="n">
-        <v>0</v>
+        <v>5588</v>
       </c>
       <c r="AL2" t="n">
         <v>0</v>
       </c>
       <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
         <v>1061.562</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AO2" t="n">
         <v>601</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AP2" t="n">
         <v>139</v>
       </c>
     </row>
@@ -783,7 +791,7 @@
         <v>0.1787200443</v>
       </c>
       <c r="E3" t="n">
-        <v>8.395435491383326</v>
+        <v>6.830238726790451</v>
       </c>
       <c r="F3" t="n">
         <v>461.1171288488211</v>
@@ -798,7 +806,7 @@
         <v>0.0340007429</v>
       </c>
       <c r="J3" t="n">
-        <v>87.27293898462972</v>
+        <v>71.00227358848048</v>
       </c>
       <c r="K3" t="n">
         <v>107.842713740458</v>
@@ -813,7 +821,7 @@
         <v>0.09557252199999999</v>
       </c>
       <c r="O3" t="n">
-        <v>4.331625523986959</v>
+        <v>3.5240621447518</v>
       </c>
       <c r="P3" t="n">
         <v>6383.531336138385</v>
@@ -825,7 +833,7 @@
         <v>0.5134428680000001</v>
       </c>
       <c r="S3" t="n">
-        <v>22.91569632044714</v>
+        <v>18.64342553997727</v>
       </c>
       <c r="T3" t="n">
         <v>0.3082933092</v>
@@ -879,18 +887,21 @@
         <v>1581</v>
       </c>
       <c r="AK3" t="n">
-        <v>0</v>
+        <v>10556</v>
       </c>
       <c r="AL3" t="n">
         <v>0</v>
       </c>
       <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
         <v>2060.9667</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="AO3" t="n">
         <v>1143</v>
       </c>
-      <c r="AO3" t="n">
+      <c r="AP3" t="n">
         <v>282</v>
       </c>
     </row>
@@ -910,7 +921,7 @@
         <v>0.0648872843</v>
       </c>
       <c r="E4" t="n">
-        <v>12.32680363115146</v>
+        <v>7.439446366782007</v>
       </c>
       <c r="F4" t="n">
         <v>354.4292042635659</v>
@@ -925,7 +936,7 @@
         <v>0.0121376796</v>
       </c>
       <c r="J4" t="n">
-        <v>86.19206880076446</v>
+        <v>52.01845444059977</v>
       </c>
       <c r="K4" t="n">
         <v>98.40825000000001</v>
@@ -940,7 +951,7 @@
         <v>0.0086080151</v>
       </c>
       <c r="O4" t="n">
-        <v>1.48112756808409</v>
+        <v>0.8938869665513265</v>
       </c>
       <c r="P4" t="n">
         <v>16056.89789210767</v>
@@ -952,7 +963,7 @@
         <v>0.3767410863</v>
       </c>
       <c r="S4" t="n">
-        <v>65.69517439082657</v>
+        <v>39.6482122260669</v>
       </c>
       <c r="T4" t="n">
         <v>0.085632979</v>
@@ -1006,18 +1017,21 @@
         <v>113</v>
       </c>
       <c r="AK4" t="n">
-        <v>0</v>
+        <v>3468</v>
       </c>
       <c r="AL4" t="n">
         <v>0</v>
       </c>
       <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
         <v>1008.7943</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AO4" t="n">
         <v>654</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="AP4" t="n">
         <v>113</v>
       </c>
     </row>
@@ -1037,7 +1051,7 @@
         <v>0.07198542049999999</v>
       </c>
       <c r="E5" t="n">
-        <v>9.764424718333903</v>
+        <v>6.598984771573605</v>
       </c>
       <c r="F5" t="n">
         <v>362.8028793706294</v>
@@ -1052,7 +1066,7 @@
         <v>0.0173194865</v>
       </c>
       <c r="J5" t="n">
-        <v>87.64083304882212</v>
+        <v>59.22934933087218</v>
       </c>
       <c r="K5" t="n">
         <v>107.6403907692308</v>
@@ -1067,7 +1081,7 @@
         <v>0.0208734778</v>
       </c>
       <c r="O5" t="n">
-        <v>2.594742232843974</v>
+        <v>1.753576372865713</v>
       </c>
       <c r="P5" t="n">
         <v>12752.04753228512</v>
@@ -1079,7 +1093,7 @@
         <v>0.3646805017</v>
       </c>
       <c r="S5" t="n">
-        <v>47.96858996244452</v>
+        <v>32.41808952468851</v>
       </c>
       <c r="T5" t="n">
         <v>0.1101783848</v>
@@ -1133,18 +1147,21 @@
         <v>227</v>
       </c>
       <c r="AK5" t="n">
-        <v>0</v>
+        <v>4334</v>
       </c>
       <c r="AL5" t="n">
         <v>0</v>
       </c>
       <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
         <v>1204.8159</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AO5" t="n">
         <v>704</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="AP5" t="n">
         <v>157</v>
       </c>
     </row>
@@ -1164,7 +1181,7 @@
         <v>0.03369626279999999</v>
       </c>
       <c r="E6" t="n">
-        <v>5.543430816237451</v>
+        <v>4.478138222849084</v>
       </c>
       <c r="F6" t="n">
         <v>515.8239299212597</v>
@@ -1179,7 +1196,7 @@
         <v>0.016135391</v>
       </c>
       <c r="J6" t="n">
-        <v>91.05194238323875</v>
+        <v>73.5543018335684</v>
       </c>
       <c r="K6" t="n">
         <v>105.5649557377049</v>
@@ -1194,7 +1211,7 @@
         <v>0.0225819015</v>
       </c>
       <c r="O6" t="n">
-        <v>3.404626800523789</v>
+        <v>2.750352609308885</v>
       </c>
       <c r="P6" t="n">
         <v>7526.215191922776</v>
@@ -1206,7 +1223,7 @@
         <v>0.1481589063</v>
       </c>
       <c r="S6" t="n">
-        <v>23.78873854212134</v>
+        <v>19.21720733427362</v>
       </c>
       <c r="T6" t="n">
         <v>0.07241355529999999</v>
@@ -1260,18 +1277,21 @@
         <v>410</v>
       </c>
       <c r="AK6" t="n">
-        <v>0</v>
+        <v>2836</v>
       </c>
       <c r="AL6" t="n">
         <v>0</v>
       </c>
       <c r="AM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" t="n">
         <v>750.1661999999999</v>
       </c>
-      <c r="AN6" t="n">
+      <c r="AO6" t="n">
         <v>408</v>
       </c>
-      <c r="AO6" t="n">
+      <c r="AP6" t="n">
         <v>98</v>
       </c>
     </row>
@@ -1291,7 +1311,7 @@
         <v>0.07287951310000002</v>
       </c>
       <c r="E7" t="n">
-        <v>8.667687595712097</v>
+        <v>7.164556962025316</v>
       </c>
       <c r="F7" t="n">
         <v>473.0905759717314</v>
@@ -1306,7 +1326,7 @@
         <v>0.0124344942</v>
       </c>
       <c r="J7" t="n">
-        <v>87.16692189892802</v>
+        <v>72.05063291139241</v>
       </c>
       <c r="K7" t="n">
         <v>102.80255</v>
@@ -1321,7 +1341,7 @@
         <v>0.035160573</v>
       </c>
       <c r="O7" t="n">
-        <v>4.165390505359878</v>
+        <v>3.443037974683544</v>
       </c>
       <c r="P7" t="n">
         <v>5685.846742891703</v>
@@ -1333,7 +1353,7 @@
         <v>0.1803775956</v>
       </c>
       <c r="S7" t="n">
-        <v>20.98009188361409</v>
+        <v>17.34177215189873</v>
       </c>
       <c r="T7" t="n">
         <v>0.1204745803</v>
@@ -1387,18 +1407,21 @@
         <v>602</v>
       </c>
       <c r="AK7" t="n">
-        <v>0</v>
+        <v>3950</v>
       </c>
       <c r="AL7" t="n">
         <v>0</v>
       </c>
       <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
         <v>686.7025</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="AO7" t="n">
         <v>399</v>
       </c>
-      <c r="AO7" t="n">
+      <c r="AP7" t="n">
         <v>99</v>
       </c>
     </row>
@@ -1418,7 +1441,7 @@
         <v>0.1411053909</v>
       </c>
       <c r="E8" t="n">
-        <v>10.68917018284107</v>
+        <v>8.49976034510305</v>
       </c>
       <c r="F8" t="n">
         <v>389.4791736842105</v>
@@ -1433,7 +1456,7 @@
         <v>0.0247043226</v>
       </c>
       <c r="J8" t="n">
-        <v>86.07594936708861</v>
+        <v>68.44543856846141</v>
       </c>
       <c r="K8" t="n">
         <v>96.8999373493976</v>
@@ -1448,7 +1471,7 @@
         <v>0.0433528176</v>
       </c>
       <c r="O8" t="n">
-        <v>3.234880450070324</v>
+        <v>2.572295893912766</v>
       </c>
       <c r="P8" t="n">
         <v>6129.204849730373</v>
@@ -1460,7 +1483,7 @@
         <v>0.3510467733</v>
       </c>
       <c r="S8" t="n">
-        <v>25.75848904962829</v>
+        <v>20.48250519252277</v>
       </c>
       <c r="T8" t="n">
         <v>0.2091625311</v>
@@ -1514,18 +1537,21 @@
         <v>622</v>
       </c>
       <c r="AK8" t="n">
-        <v>0</v>
+        <v>6259</v>
       </c>
       <c r="AL8" t="n">
         <v>0</v>
       </c>
       <c r="AM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN8" t="n">
         <v>1200.5229</v>
       </c>
-      <c r="AN8" t="n">
+      <c r="AO8" t="n">
         <v>811</v>
       </c>
-      <c r="AO8" t="n">
+      <c r="AP8" t="n">
         <v>135</v>
       </c>
     </row>
@@ -1545,7 +1571,7 @@
         <v>0.1024667677</v>
       </c>
       <c r="E9" t="n">
-        <v>9.432122836948574</v>
+        <v>7.054320087495443</v>
       </c>
       <c r="F9" t="n">
         <v>394.6645640826873</v>
@@ -1560,7 +1586,7 @@
         <v>0.0261795822</v>
       </c>
       <c r="J9" t="n">
-        <v>87.25322934438215</v>
+        <v>65.25701786365293</v>
       </c>
       <c r="K9" t="n">
         <v>103.4036894230769</v>
@@ -1575,7 +1601,7 @@
         <v>0.0372894936</v>
       </c>
       <c r="O9" t="n">
-        <v>3.314647818669266</v>
+        <v>2.479037550127598</v>
       </c>
       <c r="P9" t="n">
         <v>8334.546477898248</v>
@@ -1587,7 +1613,7 @@
         <v>0.3692541371</v>
       </c>
       <c r="S9" t="n">
-        <v>33.70704362661468</v>
+        <v>25.20962449872403</v>
       </c>
       <c r="T9" t="n">
         <v>0.1659358435</v>
@@ -1641,18 +1667,21 @@
         <v>497</v>
       </c>
       <c r="AK9" t="n">
-        <v>0</v>
+        <v>5486</v>
       </c>
       <c r="AL9" t="n">
         <v>0</v>
       </c>
       <c r="AM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="n">
         <v>1180.2412</v>
       </c>
-      <c r="AN9" t="n">
+      <c r="AO9" t="n">
         <v>696</v>
       </c>
-      <c r="AO9" t="n">
+      <c r="AP9" t="n">
         <v>153</v>
       </c>
     </row>
@@ -1672,7 +1701,7 @@
         <v>0.0391668447</v>
       </c>
       <c r="E10" t="n">
-        <v>3.625304136253042</v>
+        <v>3.311847077128251</v>
       </c>
       <c r="F10" t="n">
         <v>713.8176677852348</v>
@@ -1687,7 +1716,7 @@
         <v>0.0169706076</v>
       </c>
       <c r="J10" t="n">
-        <v>92.94403892944038</v>
+        <v>84.90775727939543</v>
       </c>
       <c r="K10" t="n">
         <v>110.4134956521739</v>
@@ -1702,7 +1731,7 @@
         <v>0.0416439843</v>
       </c>
       <c r="O10" t="n">
-        <v>3.43065693430657</v>
+        <v>3.134029784396533</v>
       </c>
       <c r="P10" t="n">
         <v>3978.26022531561</v>
@@ -1714,7 +1743,7 @@
         <v>0.1034640729</v>
       </c>
       <c r="S10" t="n">
-        <v>9.464720194647203</v>
+        <v>8.646365859079795</v>
       </c>
       <c r="T10" t="n">
         <v>0.09778143659999999</v>
@@ -1768,18 +1797,21 @@
         <v>726</v>
       </c>
       <c r="AK10" t="n">
-        <v>0</v>
+        <v>4499</v>
       </c>
       <c r="AL10" t="n">
         <v>0</v>
       </c>
       <c r="AM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="n">
         <v>472.7692000000001</v>
       </c>
-      <c r="AN10" t="n">
+      <c r="AO10" t="n">
         <v>249</v>
       </c>
-      <c r="AO10" t="n">
+      <c r="AP10" t="n">
         <v>65</v>
       </c>
     </row>
@@ -1799,7 +1831,7 @@
         <v>0.0490935509</v>
       </c>
       <c r="E11" t="n">
-        <v>5.573202425642506</v>
+        <v>5.022118136872235</v>
       </c>
       <c r="F11" t="n">
         <v>694.2430544041451</v>
@@ -1814,7 +1846,7 @@
         <v>0.0161440091</v>
       </c>
       <c r="J11" t="n">
-        <v>90.70170372509385</v>
+        <v>81.73302107728337</v>
       </c>
       <c r="K11" t="n">
         <v>101.6394971428571</v>
@@ -1829,7 +1861,7 @@
         <v>0.037019707</v>
       </c>
       <c r="O11" t="n">
-        <v>3.725093849263645</v>
+        <v>3.356752537080406</v>
       </c>
       <c r="P11" t="n">
         <v>3716.1173102739</v>
@@ -1841,7 +1873,7 @@
         <v>0.09935235399999999</v>
       </c>
       <c r="S11" t="n">
-        <v>10.97314467224949</v>
+        <v>9.888108248763986</v>
       </c>
       <c r="T11" t="n">
         <v>0.102257267</v>
@@ -1895,18 +1927,21 @@
         <v>635</v>
       </c>
       <c r="AK11" t="n">
-        <v>0</v>
+        <v>3843</v>
       </c>
       <c r="AL11" t="n">
         <v>0</v>
       </c>
       <c r="AM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="n">
         <v>289.1562</v>
       </c>
-      <c r="AN11" t="n">
+      <c r="AO11" t="n">
         <v>153</v>
       </c>
-      <c r="AO11" t="n">
+      <c r="AP11" t="n">
         <v>41</v>
       </c>
     </row>
@@ -1926,7 +1961,7 @@
         <v>0.05876800230000001</v>
       </c>
       <c r="E12" t="n">
-        <v>4.19172932330827</v>
+        <v>3.722871452420701</v>
       </c>
       <c r="F12" t="n">
         <v>548.0896291479821</v>
@@ -1941,7 +1976,7 @@
         <v>0.0236838399</v>
       </c>
       <c r="J12" t="n">
-        <v>91.65413533834587</v>
+        <v>81.40233722871453</v>
       </c>
       <c r="K12" t="n">
         <v>102.5019123595506</v>
@@ -1956,7 +1991,7 @@
         <v>0.058407151</v>
       </c>
       <c r="O12" t="n">
-        <v>4.154135338345865</v>
+        <v>3.689482470784641</v>
       </c>
       <c r="P12" t="n">
         <v>4756.529808847164</v>
@@ -1968,7 +2003,7 @@
         <v>0.1752246928</v>
       </c>
       <c r="S12" t="n">
-        <v>12.59398496240602</v>
+        <v>11.18530884808013</v>
       </c>
       <c r="T12" t="n">
         <v>0.1408589932</v>
@@ -2022,18 +2057,21 @@
         <v>1325</v>
       </c>
       <c r="AK12" t="n">
-        <v>0</v>
+        <v>5990</v>
       </c>
       <c r="AL12" t="n">
         <v>0</v>
       </c>
       <c r="AM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="n">
         <v>948.4011999999999</v>
       </c>
-      <c r="AN12" t="n">
+      <c r="AO12" t="n">
         <v>476</v>
       </c>
-      <c r="AO12" t="n">
+      <c r="AP12" t="n">
         <v>152</v>
       </c>
     </row>
@@ -2053,7 +2091,7 @@
         <v>0.06235999799999999</v>
       </c>
       <c r="E13" t="n">
-        <v>3.517376681614349</v>
+        <v>3.115303462827355</v>
       </c>
       <c r="F13" t="n">
         <v>620.3483047808766</v>
@@ -2068,7 +2106,7 @@
         <v>0.0398807475</v>
       </c>
       <c r="J13" t="n">
-        <v>93.13340807174887</v>
+        <v>82.48727814322949</v>
       </c>
       <c r="K13" t="n">
         <v>115.3086466216216</v>
@@ -2083,7 +2121,7 @@
         <v>0.0581722987</v>
       </c>
       <c r="O13" t="n">
-        <v>3.349215246636771</v>
+        <v>2.96636465185553</v>
       </c>
       <c r="P13" t="n">
         <v>5741.428351996826</v>
@@ -2095,7 +2133,7 @@
         <v>0.2411233266</v>
       </c>
       <c r="S13" t="n">
-        <v>12.90639013452915</v>
+        <v>11.43105374208763</v>
       </c>
       <c r="T13" t="n">
         <v>0.1604130442</v>
@@ -2149,18 +2187,21 @@
         <v>1303</v>
       </c>
       <c r="AK13" t="n">
-        <v>0</v>
+        <v>8057</v>
       </c>
       <c r="AL13" t="n">
         <v>0</v>
       </c>
       <c r="AM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN13" t="n">
         <v>1380.4948</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AO13" t="n">
         <v>723</v>
       </c>
-      <c r="AO13" t="n">
+      <c r="AP13" t="n">
         <v>201</v>
       </c>
     </row>
@@ -2180,7 +2221,7 @@
         <v>0.0561346029</v>
       </c>
       <c r="E14" t="n">
-        <v>4.165124028137726</v>
+        <v>3.704313467237405</v>
       </c>
       <c r="F14" t="n">
         <v>654.081516</v>
@@ -2195,7 +2236,7 @@
         <v>0.0253203807</v>
       </c>
       <c r="J14" t="n">
-        <v>91.85486856719733</v>
+        <v>81.69245966414225</v>
       </c>
       <c r="K14" t="n">
         <v>105.9784552941177</v>
@@ -2210,7 +2251,7 @@
         <v>0.0579726347</v>
       </c>
       <c r="O14" t="n">
-        <v>3.980007404664939</v>
+        <v>3.539677313137965</v>
       </c>
       <c r="P14" t="n">
         <v>4819.705078473681</v>
@@ -2222,7 +2263,7 @@
         <v>0.1775516845</v>
       </c>
       <c r="S14" t="n">
-        <v>12.43983709737134</v>
+        <v>11.06354955548238</v>
       </c>
       <c r="T14" t="n">
         <v>0.1394276183</v>
@@ -2276,18 +2317,21 @@
         <v>1147</v>
       </c>
       <c r="AK14" t="n">
-        <v>0</v>
+        <v>6074</v>
       </c>
       <c r="AL14" t="n">
         <v>0</v>
       </c>
       <c r="AM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN14" t="n">
         <v>1021.4819</v>
       </c>
-      <c r="AN14" t="n">
+      <c r="AO14" t="n">
         <v>555</v>
       </c>
-      <c r="AO14" t="n">
+      <c r="AP14" t="n">
         <v>142</v>
       </c>
     </row>
@@ -2307,7 +2351,7 @@
         <v>0.1109033978</v>
       </c>
       <c r="E15" t="n">
-        <v>7.408689631296521</v>
+        <v>6.34638196915777</v>
       </c>
       <c r="F15" t="n">
         <v>551.182430140187</v>
@@ -2322,7 +2366,7 @@
         <v>0.019454959</v>
       </c>
       <c r="J15" t="n">
-        <v>88.61000519300674</v>
+        <v>75.90450771055754</v>
       </c>
       <c r="K15" t="n">
         <v>105.3480635135135</v>
@@ -2337,7 +2381,7 @@
         <v>0.0591795099</v>
       </c>
       <c r="O15" t="n">
-        <v>3.981305175696728</v>
+        <v>3.410438908659549</v>
       </c>
       <c r="P15" t="n">
         <v>5101.882894622659</v>
@@ -2349,7 +2393,7 @@
         <v>0.2515186473</v>
       </c>
       <c r="S15" t="n">
-        <v>16.73879176042929</v>
+        <v>14.33867141162515</v>
       </c>
       <c r="T15" t="n">
         <v>0.1895378667</v>
@@ -2403,18 +2447,21 @@
         <v>1237</v>
       </c>
       <c r="AK15" t="n">
-        <v>0</v>
+        <v>6744</v>
       </c>
       <c r="AL15" t="n">
         <v>0</v>
       </c>
       <c r="AM15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN15" t="n">
         <v>1199.6448</v>
       </c>
-      <c r="AN15" t="n">
+      <c r="AO15" t="n">
         <v>627</v>
       </c>
-      <c r="AO15" t="n">
+      <c r="AP15" t="n">
         <v>173</v>
       </c>
     </row>
@@ -2434,7 +2481,7 @@
         <v>0.0227335189</v>
       </c>
       <c r="E16" t="n">
-        <v>5.328798185941043</v>
+        <v>4.276615104640583</v>
       </c>
       <c r="F16" t="n">
         <v>627.6517861702127</v>
@@ -2449,7 +2496,7 @@
         <v>0.0050523084</v>
       </c>
       <c r="J16" t="n">
-        <v>90.9297052154195</v>
+        <v>72.97543221110099</v>
       </c>
       <c r="K16" t="n">
         <v>106.11245</v>
@@ -2464,7 +2511,7 @@
         <v>0.0166687726</v>
       </c>
       <c r="O16" t="n">
-        <v>3.741496598639456</v>
+        <v>3.002729754322111</v>
       </c>
       <c r="P16" t="n">
         <v>9762.769229197358</v>
@@ -2476,7 +2523,7 @@
         <v>0.1103154519</v>
       </c>
       <c r="S16" t="n">
-        <v>24.6031746031746</v>
+        <v>19.74522292993631</v>
       </c>
       <c r="T16" t="n">
         <v>0.0444545999</v>
@@ -2530,18 +2577,21 @@
         <v>342</v>
       </c>
       <c r="AK16" t="n">
-        <v>0</v>
+        <v>2198</v>
       </c>
       <c r="AL16" t="n">
         <v>0</v>
       </c>
       <c r="AM16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN16" t="n">
         <v>379.4402</v>
       </c>
-      <c r="AN16" t="n">
+      <c r="AO16" t="n">
         <v>220</v>
       </c>
-      <c r="AO16" t="n">
+      <c r="AP16" t="n">
         <v>51</v>
       </c>
     </row>
@@ -2561,7 +2611,7 @@
         <v>0.0465223308</v>
       </c>
       <c r="E17" t="n">
-        <v>8.49956634865568</v>
+        <v>6.163522012578617</v>
       </c>
       <c r="F17" t="n">
         <v>546.8846137755102</v>
@@ -2576,7 +2626,7 @@
         <v>0.008260348299999999</v>
       </c>
       <c r="J17" t="n">
-        <v>88.3347788378144</v>
+        <v>64.05660377358491</v>
       </c>
       <c r="K17" t="n">
         <v>110.0678575757576</v>
@@ -2591,7 +2641,7 @@
         <v>0.0184477881</v>
       </c>
       <c r="O17" t="n">
-        <v>3.165654813529923</v>
+        <v>2.295597484276729</v>
       </c>
       <c r="P17" t="n">
         <v>11934.92317361591</v>
@@ -2603,7 +2653,7 @@
         <v>0.2194314667</v>
       </c>
       <c r="S17" t="n">
-        <v>37.90112749349523</v>
+        <v>27.48427672955975</v>
       </c>
       <c r="T17" t="n">
         <v>0.0732304672</v>
@@ -2657,18 +2707,21 @@
         <v>289</v>
       </c>
       <c r="AK17" t="n">
-        <v>0</v>
+        <v>3180</v>
       </c>
       <c r="AL17" t="n">
         <v>0</v>
       </c>
       <c r="AM17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN17" t="n">
         <v>714.6559</v>
       </c>
-      <c r="AN17" t="n">
+      <c r="AO17" t="n">
         <v>453</v>
       </c>
-      <c r="AO17" t="n">
+      <c r="AP17" t="n">
         <v>84</v>
       </c>
     </row>
@@ -2688,7 +2741,7 @@
         <v>0.0333299569</v>
       </c>
       <c r="E18" t="n">
-        <v>4.358578052550232</v>
+        <v>3.634957463263728</v>
       </c>
       <c r="F18" t="n">
         <v>588.7200822695035</v>
@@ -2703,7 +2756,7 @@
         <v>0.0137977969</v>
       </c>
       <c r="J18" t="n">
-        <v>91.65378670788253</v>
+        <v>76.43722608919825</v>
       </c>
       <c r="K18" t="n">
         <v>113.2173038461539</v>
@@ -2718,7 +2771,7 @@
         <v>0.0326994144</v>
       </c>
       <c r="O18" t="n">
-        <v>3.987635239567233</v>
+        <v>3.325599381283836</v>
       </c>
       <c r="P18" t="n">
         <v>8067.428853125722</v>
@@ -2730,7 +2783,7 @@
         <v>0.1602366266</v>
       </c>
       <c r="S18" t="n">
-        <v>19.90726429675425</v>
+        <v>16.60221706625419</v>
       </c>
       <c r="T18" t="n">
         <v>0.07982716819999999</v>
@@ -2784,18 +2837,21 @@
         <v>622</v>
       </c>
       <c r="AK18" t="n">
-        <v>0</v>
+        <v>3879</v>
       </c>
       <c r="AL18" t="n">
         <v>0</v>
       </c>
       <c r="AM18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN18" t="n">
         <v>656.5455999999999</v>
       </c>
-      <c r="AN18" t="n">
+      <c r="AO18" t="n">
         <v>372</v>
       </c>
-      <c r="AO18" t="n">
+      <c r="AP18" t="n">
         <v>90</v>
       </c>
     </row>
@@ -2909,7 +2965,7 @@
         <v>88</v>
       </c>
       <c r="AK19" t="n">
-        <v>0</v>
+        <v>47599</v>
       </c>
       <c r="AL19" t="n">
         <v>0</v>
@@ -2921,6 +2977,9 @@
         <v>0</v>
       </c>
       <c r="AO19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3034,7 +3093,7 @@
         <v>1059</v>
       </c>
       <c r="AK20" t="n">
-        <v>0</v>
+        <v>100070</v>
       </c>
       <c r="AL20" t="n">
         <v>0</v>
@@ -3046,6 +3105,9 @@
         <v>0</v>
       </c>
       <c r="AO20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3159,7 +3221,7 @@
         <v>2491</v>
       </c>
       <c r="AK21" t="n">
-        <v>0</v>
+        <v>100385</v>
       </c>
       <c r="AL21" t="n">
         <v>0</v>
@@ -3171,6 +3233,9 @@
         <v>0</v>
       </c>
       <c r="AO21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3284,7 +3349,7 @@
         <v>4792</v>
       </c>
       <c r="AK22" t="n">
-        <v>0</v>
+        <v>273064</v>
       </c>
       <c r="AL22" t="n">
         <v>0</v>
@@ -3296,6 +3361,9 @@
         <v>0</v>
       </c>
       <c r="AO22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3315,7 +3383,7 @@
         <v>0.0009368029</v>
       </c>
       <c r="E23" t="n">
-        <v>6.25</v>
+        <v>0.424929178470255</v>
       </c>
       <c r="F23" t="n">
         <v>542.7687333333333</v>
@@ -3330,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>93.75</v>
+        <v>6.373937677053824</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
@@ -3355,7 +3423,7 @@
         <v>0.1784866817</v>
       </c>
       <c r="S23" t="n">
-        <v>1370.833333333333</v>
+        <v>93.20113314447592</v>
       </c>
       <c r="T23" t="n">
         <v>0.0009368029</v>
@@ -3409,18 +3477,21 @@
         <v>0</v>
       </c>
       <c r="AK23" t="n">
-        <v>0</v>
+        <v>706</v>
       </c>
       <c r="AL23" t="n">
         <v>0</v>
       </c>
       <c r="AM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN23" t="n">
         <v>46.9466</v>
       </c>
-      <c r="AN23" t="n">
+      <c r="AO23" t="n">
         <v>43</v>
       </c>
-      <c r="AO23" t="n">
+      <c r="AP23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3440,7 +3511,7 @@
         <v>0.0193168294</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2888646211293902</v>
+        <v>0.282077743378053</v>
       </c>
       <c r="F24" t="n">
         <v>474.6841426829268</v>
@@ -3455,7 +3526,7 @@
         <v>0.1671950512</v>
       </c>
       <c r="J24" t="n">
-        <v>97.59044633106704</v>
+        <v>95.29755761953905</v>
       </c>
       <c r="K24" t="n">
         <v>133.9293423248882</v>
@@ -3470,7 +3541,7 @@
         <v>0.1469107566</v>
       </c>
       <c r="O24" t="n">
-        <v>2.120689047803572</v>
+        <v>2.070863433092535</v>
       </c>
       <c r="P24" t="n">
         <v>2048.451196162514</v>
@@ -3482,7 +3553,7 @@
         <v>0.1578949966</v>
       </c>
       <c r="S24" t="n">
-        <v>2.406030929650897</v>
+        <v>2.349501203990368</v>
       </c>
       <c r="T24" t="n">
         <v>0.3334226372</v>
@@ -3536,18 +3607,21 @@
         <v>4261</v>
       </c>
       <c r="AK24" t="n">
-        <v>0</v>
+        <v>29070</v>
       </c>
       <c r="AL24" t="n">
         <v>0</v>
       </c>
       <c r="AM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN24" t="n">
         <v>2671.9574</v>
       </c>
-      <c r="AN24" t="n">
+      <c r="AO24" t="n">
         <v>1842</v>
       </c>
-      <c r="AO24" t="n">
+      <c r="AP24" t="n">
         <v>270</v>
       </c>
     </row>
@@ -3567,7 +3641,7 @@
         <v>0.045729952</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6702946641890097</v>
+        <v>0.6419423523055899</v>
       </c>
       <c r="F25" t="n">
         <v>566.371953960396</v>
@@ -3582,7 +3656,7 @@
         <v>0.06645980509999999</v>
       </c>
       <c r="J25" t="n">
-        <v>97.68383328908946</v>
+        <v>93.5519750850097</v>
       </c>
       <c r="K25" t="n">
         <v>140.3962590225564</v>
@@ -3597,7 +3671,7 @@
         <v>0.1205748747</v>
       </c>
       <c r="O25" t="n">
-        <v>1.645872046721529</v>
+        <v>1.576254488829568</v>
       </c>
       <c r="P25" t="n">
         <v>5718.222694346642</v>
@@ -3609,7 +3683,7 @@
         <v>0.3211427575</v>
       </c>
       <c r="S25" t="n">
-        <v>4.416644544730555</v>
+        <v>4.22982807385515</v>
       </c>
       <c r="T25" t="n">
         <v>0.2327646318</v>
@@ -3663,18 +3737,21 @@
         <v>3179</v>
       </c>
       <c r="AK25" t="n">
-        <v>0</v>
+        <v>31467</v>
       </c>
       <c r="AL25" t="n">
         <v>0</v>
       </c>
       <c r="AM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" t="n">
         <v>3058.86</v>
       </c>
-      <c r="AN25" t="n">
+      <c r="AO25" t="n">
         <v>2768</v>
       </c>
-      <c r="AO25" t="n">
+      <c r="AP25" t="n">
         <v>92</v>
       </c>
     </row>
@@ -3694,7 +3771,7 @@
         <v>0.0402695256</v>
       </c>
       <c r="E26" t="n">
-        <v>1.089987325728771</v>
+        <v>1.027479091995221</v>
       </c>
       <c r="F26" t="n">
         <v>625.2265959302326</v>
@@ -3709,7 +3786,7 @@
         <v>0.03554541520000001</v>
       </c>
       <c r="J26" t="n">
-        <v>97.23700887198986</v>
+        <v>91.66069295101553</v>
       </c>
       <c r="K26" t="n">
         <v>141.0571106382979</v>
@@ -3724,7 +3801,7 @@
         <v>0.0662695908</v>
       </c>
       <c r="O26" t="n">
-        <v>1.673003802281369</v>
+        <v>1.577060931899642</v>
       </c>
       <c r="P26" t="n">
         <v>6756.541258851572</v>
@@ -3736,7 +3813,7 @@
         <v>0.2302864845</v>
       </c>
       <c r="S26" t="n">
-        <v>6.083650190114068</v>
+        <v>5.734767025089606</v>
       </c>
       <c r="T26" t="n">
         <v>0.1420845316</v>
@@ -3790,18 +3867,21 @@
         <v>1254</v>
       </c>
       <c r="AK26" t="n">
-        <v>0</v>
+        <v>16740</v>
       </c>
       <c r="AL26" t="n">
         <v>0</v>
       </c>
       <c r="AM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN26" t="n">
         <v>1922.4873</v>
       </c>
-      <c r="AN26" t="n">
+      <c r="AO26" t="n">
         <v>1737</v>
       </c>
-      <c r="AO26" t="n">
+      <c r="AP26" t="n">
         <v>63</v>
       </c>
     </row>
@@ -3821,7 +3901,7 @@
         <v>0.0023155657</v>
       </c>
       <c r="E27" t="n">
-        <v>0.03517298714587197</v>
+        <v>0.03482335063948335</v>
       </c>
       <c r="F27" t="n">
         <v>491.0655</v>
@@ -3836,7 +3916,7 @@
         <v>0.1523824518</v>
       </c>
       <c r="J27" t="n">
-        <v>98.99597109419965</v>
+        <v>98.01190325440039</v>
       </c>
       <c r="K27" t="n">
         <v>147.6202915625</v>
@@ -3851,7 +3931,7 @@
         <v>0.07145621059999999</v>
       </c>
       <c r="O27" t="n">
-        <v>0.9688559186544734</v>
+        <v>0.959225022160314</v>
       </c>
       <c r="P27" t="n">
         <v>1388.433029256286</v>
@@ -3863,7 +3943,7 @@
         <v>0.06926201159999999</v>
       </c>
       <c r="S27" t="n">
-        <v>1.004028905800345</v>
+        <v>0.9940483727997974</v>
       </c>
       <c r="T27" t="n">
         <v>0.2261542281</v>
@@ -3917,18 +3997,21 @@
         <v>2955</v>
       </c>
       <c r="AK27" t="n">
-        <v>0</v>
+        <v>31588</v>
       </c>
       <c r="AL27" t="n">
         <v>0</v>
       </c>
       <c r="AM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" t="n">
         <v>1512.8756</v>
       </c>
-      <c r="AN27" t="n">
+      <c r="AO27" t="n">
         <v>1297</v>
       </c>
-      <c r="AO27" t="n">
+      <c r="AP27" t="n">
         <v>73</v>
       </c>
     </row>
@@ -3948,7 +4031,7 @@
         <v>0.0123614164</v>
       </c>
       <c r="E28" t="n">
-        <v>3.458425312729949</v>
+        <v>1.998299319727891</v>
       </c>
       <c r="F28" t="n">
         <v>656.2840425531915</v>
@@ -3963,7 +4046,7 @@
         <v>0.0077710886</v>
       </c>
       <c r="J28" t="n">
-        <v>95.58498896247241</v>
+        <v>55.22959183673469</v>
       </c>
       <c r="K28" t="n">
         <v>113.5751838709678</v>
@@ -3978,7 +4061,7 @@
         <v>0.003588069499999999</v>
       </c>
       <c r="O28" t="n">
-        <v>0.9565857247976454</v>
+        <v>0.5527210884353742</v>
       </c>
       <c r="P28" t="n">
         <v>41862.39249812436</v>
@@ -3990,7 +4073,7 @@
         <v>0.2214875383</v>
       </c>
       <c r="S28" t="n">
-        <v>73.06843267108167</v>
+        <v>42.21938775510204</v>
       </c>
       <c r="T28" t="n">
         <v>0.0237205745</v>
@@ -4044,18 +4127,21 @@
         <v>27</v>
       </c>
       <c r="AK28" t="n">
-        <v>0</v>
+        <v>2352</v>
       </c>
       <c r="AL28" t="n">
         <v>0</v>
       </c>
       <c r="AM28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN28" t="n">
         <v>723.9007999999999</v>
       </c>
-      <c r="AN28" t="n">
+      <c r="AO28" t="n">
         <v>628</v>
       </c>
-      <c r="AO28" t="n">
+      <c r="AP28" t="n">
         <v>33</v>
       </c>
     </row>
@@ -4075,7 +4161,7 @@
         <v>0.02918062</v>
       </c>
       <c r="E29" t="n">
-        <v>5.4575986565911</v>
+        <v>3.54997269251775</v>
       </c>
       <c r="F29" t="n">
         <v>686.2793961538461</v>
@@ -4090,7 +4176,7 @@
         <v>0.0075150998</v>
       </c>
       <c r="J29" t="n">
-        <v>93.1150293870697</v>
+        <v>60.56799563080284</v>
       </c>
       <c r="K29" t="n">
         <v>124.6015892857143</v>
@@ -4105,7 +4191,7 @@
         <v>0.0089162151</v>
       </c>
       <c r="O29" t="n">
-        <v>1.427371956339211</v>
+        <v>0.9284543965046422</v>
       </c>
       <c r="P29" t="n">
         <v>28062.83054657258</v>
@@ -4117,7 +4203,7 @@
         <v>0.2876735221</v>
       </c>
       <c r="S29" t="n">
-        <v>53.73635600335852</v>
+        <v>34.95357728017477</v>
       </c>
       <c r="T29" t="n">
         <v>0.0456119349</v>
@@ -4171,18 +4257,21 @@
         <v>51</v>
       </c>
       <c r="AK29" t="n">
-        <v>0</v>
+        <v>3662</v>
       </c>
       <c r="AL29" t="n">
         <v>0</v>
       </c>
       <c r="AM29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN29" t="n">
         <v>1011.9574</v>
       </c>
-      <c r="AN29" t="n">
+      <c r="AO29" t="n">
         <v>935</v>
       </c>
-      <c r="AO29" t="n">
+      <c r="AP29" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4202,7 +4291,7 @@
         <v>0.0574782774</v>
       </c>
       <c r="E30" t="n">
-        <v>14.59183673469388</v>
+        <v>7.02012763868434</v>
       </c>
       <c r="F30" t="n">
         <v>643.9522748251749</v>
@@ -4217,7 +4306,7 @@
         <v>0.0018538018</v>
       </c>
       <c r="J30" t="n">
-        <v>84.43877551020408</v>
+        <v>40.62346588119784</v>
       </c>
       <c r="K30" t="n">
         <v>115.6295222222222</v>
@@ -4232,7 +4321,7 @@
         <v>0.0042492797</v>
       </c>
       <c r="O30" t="n">
-        <v>0.9693877551020408</v>
+        <v>0.4663721158566519</v>
       </c>
       <c r="P30" t="n">
         <v>33248.7388846922</v>
@@ -4244,7 +4333,7 @@
         <v>0.467561015</v>
       </c>
       <c r="S30" t="n">
-        <v>107.8571428571428</v>
+        <v>51.89003436426118</v>
       </c>
       <c r="T30" t="n">
         <v>0.0635813589</v>
@@ -4298,18 +4387,21 @@
         <v>30</v>
       </c>
       <c r="AK30" t="n">
-        <v>0</v>
+        <v>4074</v>
       </c>
       <c r="AL30" t="n">
         <v>0</v>
       </c>
       <c r="AM30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN30" t="n">
         <v>693.6256999999999</v>
       </c>
-      <c r="AN30" t="n">
+      <c r="AO30" t="n">
         <v>666</v>
       </c>
-      <c r="AO30" t="n">
+      <c r="AP30" t="n">
         <v>11</v>
       </c>
     </row>
@@ -4329,7 +4421,7 @@
         <v>0.0469265569</v>
       </c>
       <c r="E31" t="n">
-        <v>8.031088082901555</v>
+        <v>3.951921325805864</v>
       </c>
       <c r="F31" t="n">
         <v>609.6857138248847</v>
@@ -4344,7 +4436,7 @@
         <v>0.0065826593</v>
       </c>
       <c r="J31" t="n">
-        <v>91.19170984455958</v>
+        <v>44.87342924786014</v>
       </c>
       <c r="K31" t="n">
         <v>122.7694884615385</v>
@@ -4359,7 +4451,7 @@
         <v>0.0052144059</v>
       </c>
       <c r="O31" t="n">
-        <v>0.7772020725388601</v>
+        <v>0.3824439992715352</v>
       </c>
       <c r="P31" t="n">
         <v>47493.66439370231</v>
@@ -4371,7 +4463,7 @@
         <v>0.6368914766</v>
       </c>
       <c r="S31" t="n">
-        <v>103.219837157661</v>
+        <v>50.79220542706246</v>
       </c>
       <c r="T31" t="n">
         <v>0.0587236221</v>
@@ -4425,18 +4517,21 @@
         <v>40</v>
       </c>
       <c r="AK31" t="n">
-        <v>0</v>
+        <v>5491</v>
       </c>
       <c r="AL31" t="n">
         <v>0</v>
       </c>
       <c r="AM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" t="n">
         <v>1396.5928</v>
       </c>
-      <c r="AN31" t="n">
+      <c r="AO31" t="n">
         <v>1337</v>
       </c>
-      <c r="AO31" t="n">
+      <c r="AP31" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4456,7 +4551,7 @@
         <v>0.0156306536</v>
       </c>
       <c r="E32" t="n">
-        <v>5.219364599092285</v>
+        <v>2.513661202185792</v>
       </c>
       <c r="F32" t="n">
         <v>572.1509971014493</v>
@@ -4471,7 +4566,7 @@
         <v>0.0054730304</v>
       </c>
       <c r="J32" t="n">
-        <v>94.09984871406959</v>
+        <v>45.31876138433515</v>
       </c>
       <c r="K32" t="n">
         <v>121.1755272727273</v>
@@ -4486,7 +4581,7 @@
         <v>0.0022109167</v>
       </c>
       <c r="O32" t="n">
-        <v>0.680786686838124</v>
+        <v>0.3278688524590164</v>
       </c>
       <c r="P32" t="n">
         <v>61034.71461126074</v>
@@ -4498,7 +4593,7 @@
         <v>0.3227984904</v>
       </c>
       <c r="S32" t="n">
-        <v>107.6399394856278</v>
+        <v>51.83970856102004</v>
       </c>
       <c r="T32" t="n">
         <v>0.0233146007</v>
@@ -4552,18 +4647,21 @@
         <v>25</v>
       </c>
       <c r="AK32" t="n">
-        <v>0</v>
+        <v>2745</v>
       </c>
       <c r="AL32" t="n">
         <v>0</v>
       </c>
       <c r="AM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN32" t="n">
         <v>789.3553999999999</v>
       </c>
-      <c r="AN32" t="n">
+      <c r="AO32" t="n">
         <v>727</v>
       </c>
-      <c r="AO32" t="n">
+      <c r="AP32" t="n">
         <v>22</v>
       </c>
     </row>

</xml_diff>